<commit_message>
prueba de hitorias de usuario de nico
</commit_message>
<xml_diff>
--- a/Historias Usuario.xlsx
+++ b/Historias Usuario.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daren\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NICOLAS\Desktop\manja+\ManjarrezCarbajalLuisRaul8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC8CC81-E23B-4918-A5EF-CE5B64C35DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86991A1-3C8E-49AA-AD5F-59ED0A6A6640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{300541DE-7715-4B95-A302-AA55E8D2A775}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{300541DE-7715-4B95-A302-AA55E8D2A775}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint BackLog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sprint BackLog'!$A$20:$C$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sprint BackLog'!$A$20:$C$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
   <si>
     <t>HOJA 4 DE 5</t>
   </si>
@@ -329,6 +329,18 @@
   </si>
   <si>
     <t>M-024</t>
+  </si>
+  <si>
+    <t>M-025</t>
+  </si>
+  <si>
+    <t>prueba de nico</t>
+  </si>
+  <si>
+    <t>M-026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otra prueba </t>
   </si>
 </sst>
 </file>
@@ -796,60 +808,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,8 +964,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68243A5A-975C-40FC-9611-AC57FCCEEE08}" name="Tabla13" displayName="Tabla13" ref="A20:D49" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" headerRowCellStyle="Normal 2">
-  <autoFilter ref="A20:D49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68243A5A-975C-40FC-9611-AC57FCCEEE08}" name="Tabla13" displayName="Tabla13" ref="A20:D51" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" headerRowCellStyle="Normal 2">
+  <autoFilter ref="A20:D51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{33D8CE7B-F645-4DC3-B57E-F0874B4D57FA}" name="Historia de Usuario" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{C7FCB8DC-FDD2-460F-8F6F-6F45EA3033B5}" name="Por Hacer" dataDxfId="2"/>
@@ -1283,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EAE2DA-3D5A-4C39-838B-93C82A4E5F14}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="215" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1803,48 +1815,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="40" t="s">
+      <c r="A1" s="31"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="43" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1"/>
-      <c r="G1" s="41"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="40"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="41"/>
+      <c r="G2" s="44"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="40"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="43"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="41"/>
+      <c r="G3" s="44"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="40"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="41"/>
+      <c r="G4" s="44"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1852,61 +1864,61 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
-      <c r="B6" s="42" t="s">
+      <c r="A6" s="32"/>
+      <c r="B6" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
     </row>
     <row r="14" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
@@ -2112,204 +2124,212 @@
       <c r="D30" s="18"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="45"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="28"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="45"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="28"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="45"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="28"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="43" t="s">
+      <c r="A34" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="45"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="28"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="28"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="45"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="28"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="45"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="28"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="45"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="28"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="44"/>
-      <c r="D39" s="45"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="28"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="44"/>
-      <c r="D40" s="45"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="28"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="44"/>
-      <c r="D41" s="45"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="28"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="B42" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="45"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="28"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="45"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="28"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="45"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="28"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="45"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="28"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="44" t="s">
+      <c r="B46" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="45"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="28"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="44" t="s">
+      <c r="B47" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="45"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="44" t="s">
+      <c r="B48" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="44"/>
-      <c r="D48" s="45"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="28"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="45"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="28"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="22"/>
+      <c r="A50" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="27"/>
+      <c r="D50" s="28"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="20"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="22"/>
+      <c r="A51" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="27"/>
+      <c r="D51" s="28"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="20"/>

</xml_diff>